<commit_message>
Add input validation tests
</commit_message>
<xml_diff>
--- a/test_data/input_validation/false_s_projects.xlsx
+++ b/test_data/input_validation/false_s_projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hertieschool-my.sharepoint.com/personal/234533_students_hertie-school_org/Documents/MDS/DSA/student-project-matching/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lonnychen/Dropbox/@project - HERTIE SCHOOL/MDS/COURSES/Spring 2024/Data Structures &amp; Algorithms (C9)/Project/student-project-matching/test_data/input_validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{696D6183-B410-3644-AA3E-8885C773DE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A37F38-4BFD-5341-8375-07A81A4CAC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{167CAB08-E6E9-D544-8315-BD75E8338A04}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{167CAB08-E6E9-D544-8315-BD75E8338A04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>project_name</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>s7</t>
+  </si>
+  <si>
+    <t>s10</t>
   </si>
 </sst>
 </file>
@@ -145,10 +148,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -548,7 +547,7 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>